<commit_message>
update LCOM composition calculation
</commit_message>
<xml_diff>
--- a/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/LCOM_composition_10op.xlsx
+++ b/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/LCOM_composition_10op.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D94BBDA-EC43-4AE5-B6D9-B75D5AE3C197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250949E1-75F9-495C-A1DD-C108DB020F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0A822A3D-32EB-4D0D-98BA-11227E505B6A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{0A822A3D-32EB-4D0D-98BA-11227E505B6A}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOM_composition" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Component</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>LCOM with PV</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>fom PV</t>
+  </si>
+  <si>
+    <t>fom rest after variable cost</t>
   </si>
 </sst>
 </file>
@@ -569,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30977A3C-5482-456A-A386-F1EE27A7A6D1}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -711,11 +720,11 @@
       </c>
       <c r="B12" s="3">
         <f>Calculation!C8</f>
-        <v>26.708623528844758</v>
+        <v>26.38343976424186</v>
       </c>
       <c r="C12" s="3">
         <f>Calculation!D8</f>
-        <v>147.63933561778072</v>
+        <v>145.8417920301147</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -761,11 +770,11 @@
       </c>
       <c r="B19" s="3">
         <f>SUM(B2:B5)+SUM(B8:B12)+B16</f>
-        <v>250.08438387448339</v>
+        <v>249.75920010988048</v>
       </c>
       <c r="C19" s="3">
         <f>SUM(C2:C5)+SUM(C8:C12)+C16</f>
-        <v>1382.4108997506164</v>
+        <v>1380.6133561629504</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -774,11 +783,11 @@
       </c>
       <c r="B20" s="3">
         <f>B19+B15</f>
-        <v>196.81475040960547</v>
+        <v>196.48956664500255</v>
       </c>
       <c r="C20" s="3">
         <f>C19+C15</f>
-        <v>1087.9482036530967</v>
+        <v>1086.1506600654307</v>
       </c>
     </row>
   </sheetData>
@@ -788,10 +797,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208382BA-051B-4275-B93D-9F3E1E387BEF}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -800,11 +809,14 @@
     <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
     <col min="13" max="14" width="14" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -839,7 +851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -871,15 +883,15 @@
         <v>170240000</v>
       </c>
       <c r="N2" s="2">
-        <f>M2/($G$2*$G$4)</f>
+        <f t="shared" ref="N2:N8" si="0">M2/($G$2*$G$4)</f>
         <v>98.02377246615039</v>
       </c>
       <c r="O2" s="2">
-        <f>M2/($H$2*$G$4)</f>
+        <f t="shared" ref="O2:O8" si="1">M2/($H$2*$G$4)</f>
         <v>541.85363113233132</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -902,15 +914,15 @@
         <v>81809177.961825013</v>
       </c>
       <c r="N3" s="2">
-        <f>M3/($G$2*$G$4)</f>
+        <f t="shared" si="0"/>
         <v>47.105523062574839</v>
       </c>
       <c r="O3" s="2">
-        <f>M3/($H$2*$G$4)</f>
+        <f t="shared" si="1"/>
         <v>260.38886359589975</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -918,11 +930,11 @@
         <v>2267377.0034506796</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C8" si="0">(B4*$G$4)/($G$2*$G$4)</f>
+        <f t="shared" ref="C4:C8" si="2">(B4*$G$4)/($G$2*$G$4)</f>
         <v>12.818083240635005</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D8" si="1">(B4*$G$4)/($H$2*$G$4)</f>
+        <f t="shared" ref="D4:D8" si="3">(B4*$G$4)/($H$2*$G$4)</f>
         <v>70.855515691287934</v>
       </c>
       <c r="E4" s="3"/>
@@ -939,15 +951,15 @@
         <v>3088049.7494749725</v>
       </c>
       <c r="N4" s="2">
-        <f>M4/($G$2*$G$4)</f>
+        <f t="shared" si="0"/>
         <v>1.7780914356595832</v>
       </c>
       <c r="O4" s="2">
-        <f>M4/($H$2*$G$4)</f>
+        <f t="shared" si="1"/>
         <v>9.8288943248960283</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -955,11 +967,11 @@
         <v>-193797.78581274601</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.0955902554440666</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-6.0561794675935898</v>
       </c>
       <c r="E5" s="3"/>
@@ -970,15 +982,15 @@
         <v>32920816.079183012</v>
       </c>
       <c r="N5" s="2">
-        <f>M5/($G$2*$G$4)</f>
+        <f t="shared" si="0"/>
         <v>18.955724769418591</v>
       </c>
       <c r="O5" s="2">
-        <f>M5/($H$2*$G$4)</f>
+        <f t="shared" si="1"/>
         <v>104.78303414206387</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -986,11 +998,11 @@
         <v>106705.6318900662</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.60323522278379571</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.3345502592770924</v>
       </c>
       <c r="E6" s="3"/>
@@ -1002,15 +1014,15 @@
         <v>52</v>
       </c>
       <c r="N6" s="2">
-        <f>M6/($G$2*$G$4)</f>
+        <f t="shared" si="0"/>
         <v>2.9941471852912479E-5</v>
       </c>
       <c r="O6" s="2">
-        <f>M6/($H$2*$G$4)</f>
+        <f t="shared" si="1"/>
         <v>1.6550980274248841E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1018,11 +1030,11 @@
         <v>1207697.2399275706</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.8274326357361232</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37.740530403096898</v>
       </c>
       <c r="E7" s="3"/>
@@ -1033,28 +1045,29 @@
         <v>263636.26426398754</v>
       </c>
       <c r="N7" s="2">
-        <f>M7/($G$2*$G$4)</f>
+        <f t="shared" si="0"/>
         <v>0.15180111126667653</v>
       </c>
       <c r="O7" s="2">
-        <f>M7/($H$2*$G$4)</f>
+        <f t="shared" si="1"/>
         <v>0.83912280950190621</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2">
-        <v>4724459.7843728997</v>
+        <f>E13+F14</f>
+        <v>4666938.3768492891</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="0"/>
-        <v>26.708623528844758</v>
+        <f>(B8*$G$4)/($G$2*$G$4)</f>
+        <v>26.38343976424186</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="1"/>
-        <v>147.63933561778072</v>
+        <f>(B8*$G$4)/($H$2*$G$4)</f>
+        <v>145.8417920301147</v>
       </c>
       <c r="E8" s="3"/>
       <c r="L8" t="s">
@@ -1064,36 +1077,76 @@
         <v>334376.152584158</v>
       </c>
       <c r="N8" s="2">
-        <f>M8/($G$2*$G$4)</f>
+        <f t="shared" si="0"/>
         <v>0.19253296463237954</v>
       </c>
       <c r="O8" s="2">
-        <f>M8/($H$2*$G$4)</f>
+        <f t="shared" si="1"/>
         <v>1.0642794433845422</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="10" spans="1:16">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:16">
       <c r="G11" s="1"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="12" spans="1:16">
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="3">
         <f>SUM(D3:D8)+SUM(O2:O8)</f>
-        <v>1382.411065260419</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>1380.613521672753</v>
+      </c>
+      <c r="E13">
+        <f>304*11300</f>
+        <v>3435200</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1921371.8921226684</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3">
         <f>SUM(D2:D8)+SUM(O2:O8)</f>
-        <v>1087.9483691628996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <v>1086.1508255752335</v>
+      </c>
+      <c r="F14" s="3">
+        <f>F13-SUM(B2:B7)</f>
+        <v>1231738.3768492891</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="L15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15">
+        <v>4.34</v>
+      </c>
+      <c r="P15">
+        <f>O15*8254*44</f>
+        <v>1576183.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="E16" t="s">
         <v>23</v>
       </c>
@@ -1103,18 +1156,42 @@
       <c r="G16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="5:7">
+      <c r="L16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" t="s">
+        <v>46</v>
+      </c>
+      <c r="N16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
       <c r="E17">
         <v>53440252.431568697</v>
       </c>
-    </row>
-    <row r="18" spans="5:7">
+      <c r="L17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17">
+        <v>0.1192922374429224</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
       <c r="E18" s="2">
         <v>17696835.495142099</v>
       </c>
     </row>
-    <row r="19" spans="5:7">
+    <row r="19" spans="2:15">
       <c r="E19" s="2">
         <f>SUM(E17:E18)</f>
         <v>71137087.926710799</v>
@@ -1126,8 +1203,34 @@
         <f>F19*E19</f>
         <v>106705.6318900662</v>
       </c>
-    </row>
-    <row r="22" spans="5:7">
+      <c r="L19">
+        <v>0.82802811702252499</v>
+      </c>
+      <c r="O19">
+        <f>L19*52*O15</f>
+        <v>186.86938544964343</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="L20" s="1">
+        <v>0.468957494005449</v>
+      </c>
+      <c r="O20">
+        <f>L20*52*O16</f>
+        <v>108.51676411286091</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="3"/>
+      <c r="L21" s="1">
+        <v>1.75757509509804E-2</v>
+      </c>
+      <c r="O21">
+        <f>L21*100*O17</f>
+        <v>0.2096650655682023</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15">
       <c r="E22" t="s">
         <v>27</v>
       </c>
@@ -1135,7 +1238,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="5:7">
+    <row r="23" spans="2:15">
       <c r="E23">
         <v>45046.521444519603</v>
       </c>

</xml_diff>

<commit_message>
update LCOM values part I
</commit_message>
<xml_diff>
--- a/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/LCOM_composition_10op.xlsx
+++ b/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/LCOM_composition_10op.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250949E1-75F9-495C-A1DD-C108DB020F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E256C5-E522-4E8F-9BF5-B5462AE2B8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{0A822A3D-32EB-4D0D-98BA-11227E505B6A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0A822A3D-32EB-4D0D-98BA-11227E505B6A}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOM_composition" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Component</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>fom rest after variable cost</t>
+  </si>
+  <si>
+    <t>storage</t>
+  </si>
+  <si>
+    <t>funits_on methanol</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30977A3C-5482-456A-A386-F1EE27A7A6D1}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -668,11 +674,11 @@
       </c>
       <c r="B8" s="3">
         <f>Calculation!C3</f>
-        <v>38.015153692225311</v>
+        <v>37.509953305926445</v>
       </c>
       <c r="C8" s="3">
         <f>Calculation!D3</f>
-        <v>210.13932179868991</v>
+        <v>207.34668632998228</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -681,11 +687,11 @@
       </c>
       <c r="B9" s="3">
         <f>Calculation!C4</f>
-        <v>12.818083240635005</v>
+        <v>12.821049504057514</v>
       </c>
       <c r="C9" s="3">
         <f>Calculation!D4</f>
-        <v>70.855515691287934</v>
+        <v>70.871912536317922</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -694,11 +700,11 @@
       </c>
       <c r="B10" s="3">
         <f>Calculation!C6</f>
-        <v>0.60323522278379571</v>
+        <v>0.59784438075713109</v>
       </c>
       <c r="C10" s="3">
         <f>Calculation!D6</f>
-        <v>3.3345502592770924</v>
+        <v>3.3047508825185852</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -719,12 +725,12 @@
         <v>40</v>
       </c>
       <c r="B12" s="3">
-        <f>Calculation!C8</f>
-        <v>26.38343976424186</v>
+        <f>Calculation!C9</f>
+        <v>42.315121512372421</v>
       </c>
       <c r="C12" s="3">
-        <f>Calculation!D8</f>
-        <v>145.8417920301147</v>
+        <f>Calculation!D9</f>
+        <v>233.90858836005864</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -744,11 +750,11 @@
       </c>
       <c r="B15" s="3">
         <f>Calculation!C2</f>
-        <v>-53.269633464877934</v>
+        <v>-52.309579961412652</v>
       </c>
       <c r="C15" s="3">
         <f>Calculation!D2</f>
-        <v>-294.46269609751965</v>
+        <v>-289.15573367558659</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -757,11 +763,11 @@
       </c>
       <c r="B16" s="3">
         <f>Calculation!C5</f>
-        <v>-1.0955902554440666</v>
+        <v>-19.344559304624418</v>
       </c>
       <c r="C16" s="3">
         <f>Calculation!D5</f>
-        <v>-6.0561794675935898</v>
+        <v>-106.93242504500719</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -770,11 +776,11 @@
       </c>
       <c r="B19" s="3">
         <f>SUM(B2:B5)+SUM(B8:B12)+B16</f>
-        <v>249.75920010988048</v>
+        <v>246.93428784392771</v>
       </c>
       <c r="C19" s="3">
         <f>SUM(C2:C5)+SUM(C8:C12)+C16</f>
-        <v>1380.6133561629504</v>
+        <v>1364.9978689150446</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -783,11 +789,11 @@
       </c>
       <c r="B20" s="3">
         <f>B19+B15</f>
-        <v>196.48956664500255</v>
+        <v>194.62470788251505</v>
       </c>
       <c r="C20" s="3">
         <f>C19+C15</f>
-        <v>1086.1506600654307</v>
+        <v>1075.842135239458</v>
       </c>
     </row>
   </sheetData>
@@ -797,10 +803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208382BA-051B-4275-B93D-9F3E1E387BEF}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -813,10 +819,12 @@
     <col min="7" max="7" width="11.88671875" customWidth="1"/>
     <col min="12" max="12" width="15.33203125" customWidth="1"/>
     <col min="13" max="14" width="14" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" customWidth="1"/>
+    <col min="22" max="22" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -850,21 +858,30 @@
       <c r="O1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>-9422808.3585551307</v>
+        <v>-9252985.5235045142</v>
       </c>
       <c r="C2" s="2">
         <f>(B2*$G$4)/($G$2*$G$4)</f>
-        <v>-53.269633464877934</v>
+        <v>-52.309579961412652</v>
       </c>
       <c r="D2" s="2">
         <f>(B2*$G$4)/($H$2*$G$4)</f>
-        <v>-294.46269609751965</v>
+        <v>-289.15573367558659</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -890,21 +907,24 @@
         <f t="shared" ref="O2:O8" si="1">M2/($H$2*$G$4)</f>
         <v>541.85363113233132</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="V2">
+        <v>53440252.431568697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>6724459.7843729397</v>
+        <v>6635095.4296153476</v>
       </c>
       <c r="C3" s="2">
         <f>(B3*$G$4)/($G$2*$G$4)</f>
-        <v>38.015153692225311</v>
+        <v>37.509953305926445</v>
       </c>
       <c r="D3" s="2">
         <f>(B3*$G$4)/($H$2*$G$4)</f>
-        <v>210.13932179868991</v>
+        <v>207.34668632998228</v>
       </c>
       <c r="G3" s="1"/>
       <c r="L3" t="s">
@@ -921,21 +941,24 @@
         <f t="shared" si="1"/>
         <v>260.38886359589975</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="V3" s="2">
+        <v>17696835.495142099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="2">
-        <v>2267377.0034506796</v>
+        <v>2267901.7026076526</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C8" si="2">(B4*$G$4)/($G$2*$G$4)</f>
-        <v>12.818083240635005</v>
+        <f t="shared" ref="C4:C7" si="2">(B4*$G$4)/($G$2*$G$4)</f>
+        <v>12.821049504057514</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D8" si="3">(B4*$G$4)/($H$2*$G$4)</f>
-        <v>70.855515691287934</v>
+        <v>70.871912536317922</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" t="s">
@@ -958,21 +981,32 @@
         <f t="shared" si="1"/>
         <v>9.8288943248960283</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="V4" s="2">
+        <f>SUM(V2:V3)</f>
+        <v>71137087.926710799</v>
+      </c>
+      <c r="W4">
+        <v>1.4865951742627349E-3</v>
+      </c>
+      <c r="X4">
+        <f>W4*V4</f>
+        <v>105752.05162295215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2">
-        <v>-193797.78581274601</v>
+        <v>-3421838.35802742</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="2"/>
-        <v>-1.0955902554440666</v>
+        <f>(B5*$G$4)/($G$2*$G$4)</f>
+        <v>-19.344559304624418</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="3"/>
-        <v>-6.0561794675935898</v>
+        <f>(B5*$G$4)/($H$2*$G$4)</f>
+        <v>-106.93242504500719</v>
       </c>
       <c r="E5" s="3"/>
       <c r="L5" t="s">
@@ -989,21 +1023,26 @@
         <f t="shared" si="1"/>
         <v>104.78303414206387</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="2">
+        <f>SUM(M2:M8)*0.03</f>
+        <v>8659683.246219933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="2">
-        <v>106705.6318900662</v>
+        <f>X4</f>
+        <v>105752.05162295215</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="2"/>
-        <v>0.60323522278379571</v>
+        <v>0.59784438075713109</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="3"/>
-        <v>3.3345502592770924</v>
+        <v>3.3047508825185852</v>
       </c>
       <c r="E6" s="3"/>
       <c r="H6" s="1"/>
@@ -1022,7 +1061,7 @@
         <v>1.6550980274248841E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1052,22 +1091,27 @@
         <f t="shared" si="1"/>
         <v>0.83912280950190621</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="V7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2">
-        <f>E13+F14</f>
-        <v>4666938.3768492891</v>
+        <v>329888.299992999</v>
       </c>
       <c r="C8" s="2">
         <f>(B8*$G$4)/($G$2*$G$4)</f>
-        <v>26.38343976424186</v>
+        <v>1.8649460072085511</v>
       </c>
       <c r="D8" s="2">
-        <f>(B8*$G$4)/($H$2*$G$4)</f>
-        <v>145.8417920301147</v>
+        <f t="shared" si="3"/>
+        <v>10.309007095402823</v>
       </c>
       <c r="E8" s="3"/>
       <c r="L8" t="s">
@@ -1084,51 +1128,108 @@
         <f t="shared" si="1"/>
         <v>1.0642794433845422</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="V8">
+        <v>45046.521444519603</v>
+      </c>
+      <c r="W8">
+        <v>26.81</v>
+      </c>
+      <c r="X8">
+        <f>W8*V8</f>
+        <v>1207697.2399275706</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
+        <f>E13+SUM(Q14:Q17)</f>
+        <v>7485076.4825132545</v>
+      </c>
+      <c r="C9" s="2">
+        <f>(B9*$G$4)/($G$2*$G$4)</f>
+        <v>42.315121512372421</v>
+      </c>
+      <c r="D9" s="2">
+        <f>(B9*$G$4)/($H$2*$G$4)</f>
+        <v>233.90858836005864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:24">
       <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="P11">
+        <v>38000</v>
+      </c>
+      <c r="Q11">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="E12" t="s">
         <v>47</v>
       </c>
       <c r="F12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="P12">
+        <f>P11/8760</f>
+        <v>4.3378995433789953</v>
+      </c>
+      <c r="Q12">
+        <f>Q11/8760</f>
+        <v>4.4520547945205475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="3">
-        <f>SUM(D3:D8)+SUM(O2:O8)</f>
-        <v>1380.613521672753</v>
+        <f>SUM(D3:D9)+SUM(O2:O8)</f>
+        <v>1375.3070415202501</v>
       </c>
       <c r="E13">
         <f>304*11300</f>
         <v>3435200</v>
       </c>
       <c r="F13" s="2">
-        <v>1921371.8921226684</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>1462147.8309085499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3">
-        <f>SUM(D2:D8)+SUM(O2:O8)</f>
-        <v>1086.1508255752335</v>
+        <f>SUM(D2:D9)+SUM(O2:O8)</f>
+        <v>1086.1513078446635</v>
       </c>
       <c r="F14" s="3">
-        <f>F13-SUM(B2:B7)</f>
-        <v>1231738.3768492891</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <f>F13-SUM(B2:B8)</f>
+        <v>3590636.9886739617</v>
+      </c>
+      <c r="L14" t="s">
+        <v>49</v>
+      </c>
+      <c r="M14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14">
+        <v>1.0958904109589039E-2</v>
+      </c>
+      <c r="Q14" s="2">
+        <f>O14*8760*1000*L19*4</f>
+        <v>383999.99999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="L15" t="s">
         <v>3</v>
       </c>
@@ -1141,21 +1242,12 @@
       <c r="O15">
         <v>4.34</v>
       </c>
-      <c r="P15">
-        <f>O15*8254*44</f>
-        <v>1576183.84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
+      <c r="Q15" s="2">
+        <f>O15*8760*52*L20</f>
+        <v>1636975.8165388766</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="L16" t="s">
         <v>6</v>
       </c>
@@ -1168,11 +1260,12 @@
       <c r="O16">
         <v>4.45</v>
       </c>
-    </row>
-    <row r="17" spans="2:15">
-      <c r="E17">
-        <v>53440252.431568697</v>
-      </c>
+      <c r="Q16" s="2">
+        <f>O16*8760*52</f>
+        <v>2027064</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17">
       <c r="L17" t="s">
         <v>7</v>
       </c>
@@ -1185,69 +1278,101 @@
       <c r="O17">
         <v>0.1192922374429224</v>
       </c>
-    </row>
-    <row r="18" spans="2:15">
-      <c r="E18" s="2">
-        <v>17696835.495142099</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15">
-      <c r="E19" s="2">
-        <f>SUM(E17:E18)</f>
-        <v>71137087.926710799</v>
-      </c>
-      <c r="F19">
-        <v>1.5E-3</v>
-      </c>
-      <c r="G19">
-        <f>F19*E19</f>
-        <v>106705.6318900662</v>
-      </c>
+      <c r="Q17" s="2">
+        <f>O17*8760*100*L22</f>
+        <v>1836.6659743774524</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
       <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <f>O14*1000</f>
+        <v>10.958904109589039</v>
+      </c>
+      <c r="P19">
+        <f>O19*174</f>
+        <v>1906.8493150684928</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17">
+      <c r="L20">
         <v>0.82802811702252499</v>
       </c>
-      <c r="O19">
-        <f>L19*52*O15</f>
+      <c r="M20">
+        <f>L20*52</f>
+        <v>43.057462085171302</v>
+      </c>
+      <c r="O20" s="2">
+        <f>L20*52*O15</f>
         <v>186.86938544964343</v>
       </c>
-    </row>
-    <row r="20" spans="2:15">
-      <c r="L20" s="1">
-        <v>0.468957494005449</v>
-      </c>
-      <c r="O20">
-        <f>L20*52*O16</f>
-        <v>108.51676411286091</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15">
+      <c r="P20" s="2">
+        <f>O20*6012.5</f>
+        <v>1123552.1800159812</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
       <c r="B21" s="3"/>
       <c r="L21" s="1">
+        <v>0.468957494005449</v>
+      </c>
+      <c r="O21" s="2">
+        <f>L21*52*O16</f>
+        <v>108.51676411286091</v>
+      </c>
+      <c r="P21" s="2">
+        <f>O21*866.9</f>
+        <v>94073.182809439124</v>
+      </c>
+      <c r="Q21" s="3">
+        <f>F14-P23</f>
+        <v>2371077.9394050804</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="L22" s="1">
         <v>1.75757509509804E-2</v>
       </c>
-      <c r="O21">
-        <f>L21*100*O17</f>
+      <c r="O22" s="2">
+        <f>L22*100*O17</f>
         <v>0.2096650655682023</v>
       </c>
-    </row>
-    <row r="22" spans="2:15">
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15">
-      <c r="E23">
-        <v>45046.521444519603</v>
-      </c>
-      <c r="F23">
-        <v>26.81</v>
-      </c>
-      <c r="G23">
-        <f>F23*E23</f>
-        <v>1207697.2399275706</v>
+      <c r="P22" s="2">
+        <f>O22*128</f>
+        <v>26.837128392729895</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
+      <c r="O23" s="2">
+        <f>SUM(O19:O22)</f>
+        <v>306.55471873766157</v>
+      </c>
+      <c r="P23" s="2">
+        <f>SUM(P19:P22)</f>
+        <v>1219559.0492688813</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17">
+      <c r="F28">
+        <v>4618681.2796730399</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17">
+      <c r="F29" s="3">
+        <f>F28-SUM(B2:B7)</f>
+        <v>7077058.7374314507</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17">
+      <c r="F30" s="3">
+        <f>B9-F29</f>
+        <v>408017.74508180376</v>
+      </c>
+      <c r="G30" s="3">
+        <f>F14-SUM(Q14:Q17)</f>
+        <v>-459239.49383929279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update LCOM composition file
</commit_message>
<xml_diff>
--- a/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/LCOM_composition_10op.xlsx
+++ b/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/LCOM_composition_10op.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\Nord_H2ub\Spine_Projects\03_output_data\03_runs_paper_energy_2024\03_results_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E256C5-E522-4E8F-9BF5-B5462AE2B8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2E4874-D3DF-4183-AC19-A98B3DD7301E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0A822A3D-32EB-4D0D-98BA-11227E505B6A}"/>
   </bookViews>
@@ -585,7 +585,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -729,8 +729,8 @@
         <v>42.315121512372421</v>
       </c>
       <c r="C12" s="3">
-        <f>Calculation!D9</f>
-        <v>233.90858836005864</v>
+        <f>Calculation!D9+Calculation!D8</f>
+        <v>244.21759545546146</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -746,7 +746,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3">
         <f>Calculation!C2</f>
@@ -759,7 +759,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3">
         <f>Calculation!C5</f>
@@ -780,7 +780,7 @@
       </c>
       <c r="C19" s="3">
         <f>SUM(C2:C5)+SUM(C8:C12)+C16</f>
-        <v>1364.9978689150446</v>
+        <v>1375.3068760104475</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -793,7 +793,7 @@
       </c>
       <c r="C20" s="3">
         <f>C19+C15</f>
-        <v>1075.842135239458</v>
+        <v>1086.1511423348609</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +806,7 @@
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>